<commit_message>
Xamarin Studio Build improvements + REST API coverage update + Unit test fix
Signed-off-by: David Noble <dnoble@splunk.com>
</commit_message>
<xml_diff>
--- a/docs/REST API coverage.xlsx
+++ b/docs/REST API coverage.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="24526"/>
   <workbookPr showInkAnnotation="0" hidePivotFieldList="1" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="-440" windowWidth="51200" windowHeight="32000" tabRatio="500" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="-440" windowWidth="28800" windowHeight="18000" tabRatio="500" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet2" sheetId="2" r:id="rId1"/>
@@ -12,7 +12,7 @@
   </sheets>
   <calcPr calcId="140000" concurrentCalc="0"/>
   <pivotCaches>
-    <pivotCache cacheId="1" r:id="rId3"/>
+    <pivotCache cacheId="0" r:id="rId3"/>
   </pivotCaches>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
@@ -61,7 +61,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="590" uniqueCount="395">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="590" uniqueCount="394">
   <si>
     <t>Access Control</t>
   </si>
@@ -678,9 +678,6 @@
     <t xml:space="preserve">Use the Applications endpoints to install applications and application templates into a Splunk instance. </t>
   </si>
   <si>
-    <t>O</t>
-  </si>
-  <si>
     <t>Create events from the contents contained in the HTTP body.</t>
   </si>
   <si>
@@ -1158,12 +1155,6 @@
     <t>POST server/logger/{name}</t>
   </si>
   <si>
-    <t>1 = Must have in splunk-sdk-csharp-2.0.0</t>
-  </si>
-  <si>
-    <t>2 = Nice to have in splunk-sdk-csharp-2.0.0</t>
-  </si>
-  <si>
     <t>PCL-3</t>
   </si>
   <si>
@@ -1246,6 +1237,12 @@
   </si>
   <si>
     <t>Edit the identified credentials.</t>
+  </si>
+  <si>
+    <t>1 = Must have in splunk-sdk-csharp-pcl-2.0.0</t>
+  </si>
+  <si>
+    <t>2 = Nice to have in splunk-sdk-csharp-pcl-2.0.0</t>
   </si>
 </sst>
 </file>
@@ -1312,7 +1309,7 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -1322,12 +1319,6 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="7" tint="0.79998168889431442"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.59999389629810485"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1360,7 +1351,7 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="31">
+  <cellXfs count="30">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" indent="1"/>
@@ -1428,9 +1419,6 @@
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
@@ -3026,7 +3014,7 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="PivotTable1" cacheId="1" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="4" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="4" indent="0" outline="1" outlineData="1" gridDropZones="1" multipleFieldFilters="0">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="PivotTable1" cacheId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="4" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="4" indent="0" outline="1" outlineData="1" gridDropZones="1" multipleFieldFilters="0">
   <location ref="A3:F10" firstHeaderRow="1" firstDataRow="2" firstDataCol="1"/>
   <pivotFields count="6">
     <pivotField dataField="1" showAll="0"/>
@@ -3478,30 +3466,30 @@
   <sheetData>
     <row r="3" spans="1:6">
       <c r="A3" s="19" t="s">
-        <v>370</v>
+        <v>367</v>
       </c>
       <c r="B3" s="19" t="s">
-        <v>371</v>
+        <v>368</v>
       </c>
     </row>
     <row r="4" spans="1:6">
       <c r="A4" s="19" t="s">
-        <v>372</v>
+        <v>369</v>
       </c>
       <c r="B4" t="s">
-        <v>368</v>
+        <v>365</v>
       </c>
       <c r="C4" t="s">
-        <v>367</v>
+        <v>364</v>
       </c>
       <c r="D4" t="s">
-        <v>369</v>
+        <v>366</v>
       </c>
       <c r="E4" t="s">
-        <v>373</v>
+        <v>370</v>
       </c>
       <c r="F4" t="s">
-        <v>374</v>
+        <v>371</v>
       </c>
     </row>
     <row r="5" spans="1:6">
@@ -3568,7 +3556,7 @@
     </row>
     <row r="9" spans="1:6">
       <c r="A9" s="2" t="s">
-        <v>373</v>
+        <v>370</v>
       </c>
       <c r="B9" s="20"/>
       <c r="C9" s="20"/>
@@ -3582,7 +3570,7 @@
     </row>
     <row r="10" spans="1:6">
       <c r="A10" s="2" t="s">
-        <v>374</v>
+        <v>371</v>
       </c>
       <c r="B10" s="20">
         <v>25</v>
@@ -3614,14 +3602,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D205"/>
   <sheetViews>
-    <sheetView tabSelected="1" showRuler="0" topLeftCell="A76" workbookViewId="0">
-      <selection activeCell="G136" sqref="G136"/>
+    <sheetView tabSelected="1" showRuler="0" workbookViewId="0">
+      <selection activeCell="A209" sqref="A209:B209"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" outlineLevelRow="1" x14ac:dyDescent="0"/>
   <cols>
-    <col min="1" max="1" width="48.83203125" customWidth="1"/>
-    <col min="2" max="2" width="157.83203125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="66.1640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="132.33203125" customWidth="1"/>
     <col min="3" max="3" width="11.83203125" style="3" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="12.83203125" style="3" bestFit="1" customWidth="1"/>
   </cols>
@@ -3640,7 +3628,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:4" outlineLevel="1">
+    <row r="2" spans="1:4" hidden="1" outlineLevel="1">
       <c r="A2" s="4" t="s">
         <v>73</v>
       </c>
@@ -3654,7 +3642,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:4" outlineLevel="1">
+    <row r="3" spans="1:4" hidden="1" outlineLevel="1">
       <c r="A3" s="4" t="s">
         <v>75</v>
       </c>
@@ -3668,7 +3656,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:4" outlineLevel="1">
+    <row r="4" spans="1:4" hidden="1" outlineLevel="1">
       <c r="A4" s="4" t="s">
         <v>77</v>
       </c>
@@ -3682,7 +3670,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:4" outlineLevel="1">
+    <row r="5" spans="1:4" hidden="1" outlineLevel="1">
       <c r="A5" s="4" t="s">
         <v>79</v>
       </c>
@@ -3696,7 +3684,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:4" outlineLevel="1">
+    <row r="6" spans="1:4" hidden="1" outlineLevel="1">
       <c r="A6" s="4" t="s">
         <v>81</v>
       </c>
@@ -3710,7 +3698,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="1:4" outlineLevel="1">
+    <row r="7" spans="1:4" hidden="1" outlineLevel="1">
       <c r="A7" s="4" t="s">
         <v>83</v>
       </c>
@@ -3724,7 +3712,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="1:4" outlineLevel="1">
+    <row r="8" spans="1:4" hidden="1" outlineLevel="1">
       <c r="A8" s="4" t="s">
         <v>97</v>
       </c>
@@ -3738,7 +3726,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="9" spans="1:4" outlineLevel="1">
+    <row r="9" spans="1:4" hidden="1" outlineLevel="1">
       <c r="A9" s="7" t="s">
         <v>85</v>
       </c>
@@ -3752,7 +3740,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="10" spans="1:4" outlineLevel="1">
+    <row r="10" spans="1:4" hidden="1" outlineLevel="1">
       <c r="A10" s="4" t="s">
         <v>87</v>
       </c>
@@ -3766,7 +3754,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="11" spans="1:4" outlineLevel="1">
+    <row r="11" spans="1:4" hidden="1" outlineLevel="1">
       <c r="A11" s="4" t="s">
         <v>89</v>
       </c>
@@ -3780,7 +3768,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="12" spans="1:4" outlineLevel="1">
+    <row r="12" spans="1:4" hidden="1" outlineLevel="1">
       <c r="A12" s="12" t="s">
         <v>91</v>
       </c>
@@ -3794,7 +3782,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="13" spans="1:4" outlineLevel="1">
+    <row r="13" spans="1:4" hidden="1" outlineLevel="1">
       <c r="A13" s="13" t="s">
         <v>93</v>
       </c>
@@ -3808,7 +3796,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="14" spans="1:4" outlineLevel="1">
+    <row r="14" spans="1:4" hidden="1" outlineLevel="1">
       <c r="A14" s="13" t="s">
         <v>95</v>
       </c>
@@ -3822,7 +3810,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="15" spans="1:4">
+    <row r="15" spans="1:4" collapsed="1">
       <c r="A15" s="21" t="s">
         <v>71</v>
       </c>
@@ -3831,10 +3819,10 @@
       </c>
       <c r="C15" s="23"/>
       <c r="D15" s="24" t="s">
-        <v>379</v>
-      </c>
-    </row>
-    <row r="16" spans="1:4" outlineLevel="1">
+        <v>376</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" hidden="1" outlineLevel="1">
       <c r="A16" s="4" t="s">
         <v>123</v>
       </c>
@@ -3842,13 +3830,13 @@
         <v>124</v>
       </c>
       <c r="C16" s="3" t="s">
-        <v>385</v>
+        <v>382</v>
       </c>
       <c r="D16" s="14">
         <v>2</v>
       </c>
     </row>
-    <row r="17" spans="1:4" outlineLevel="1">
+    <row r="17" spans="1:4" hidden="1" outlineLevel="1">
       <c r="A17" s="4" t="s">
         <v>125</v>
       </c>
@@ -3856,13 +3844,13 @@
         <v>126</v>
       </c>
       <c r="C17" s="3" t="s">
-        <v>385</v>
+        <v>382</v>
       </c>
       <c r="D17" s="14">
         <v>2</v>
       </c>
     </row>
-    <row r="18" spans="1:4" outlineLevel="1">
+    <row r="18" spans="1:4" hidden="1" outlineLevel="1">
       <c r="A18" s="4" t="s">
         <v>127</v>
       </c>
@@ -3870,13 +3858,13 @@
         <v>128</v>
       </c>
       <c r="C18" s="3" t="s">
-        <v>385</v>
+        <v>382</v>
       </c>
       <c r="D18" s="14">
         <v>2</v>
       </c>
     </row>
-    <row r="19" spans="1:4" outlineLevel="1">
+    <row r="19" spans="1:4" hidden="1" outlineLevel="1">
       <c r="A19" s="13" t="s">
         <v>130</v>
       </c>
@@ -3884,13 +3872,13 @@
         <v>129</v>
       </c>
       <c r="C19" s="3" t="s">
-        <v>385</v>
+        <v>382</v>
       </c>
       <c r="D19" s="17">
         <v>2</v>
       </c>
     </row>
-    <row r="20" spans="1:4" outlineLevel="1">
+    <row r="20" spans="1:4" hidden="1" outlineLevel="1">
       <c r="A20" s="4" t="s">
         <v>131</v>
       </c>
@@ -3898,13 +3886,13 @@
         <v>132</v>
       </c>
       <c r="C20" s="3" t="s">
-        <v>385</v>
+        <v>382</v>
       </c>
       <c r="D20" s="14">
         <v>2</v>
       </c>
     </row>
-    <row r="21" spans="1:4" outlineLevel="1">
+    <row r="21" spans="1:4" hidden="1" outlineLevel="1">
       <c r="A21" s="13" t="s">
         <v>134</v>
       </c>
@@ -3918,7 +3906,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="22" spans="1:4" outlineLevel="1">
+    <row r="22" spans="1:4" hidden="1" outlineLevel="1">
       <c r="A22" s="4" t="s">
         <v>135</v>
       </c>
@@ -3932,7 +3920,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="23" spans="1:4" s="8" customFormat="1" outlineLevel="1" collapsed="1">
+    <row r="23" spans="1:4" s="8" customFormat="1" hidden="1" outlineLevel="1" collapsed="1">
       <c r="A23" s="13" t="s">
         <v>137</v>
       </c>
@@ -3946,7 +3934,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="24" spans="1:4" outlineLevel="1">
+    <row r="24" spans="1:4" hidden="1" outlineLevel="1">
       <c r="A24" s="4" t="s">
         <v>139</v>
       </c>
@@ -3960,7 +3948,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="25" spans="1:4" outlineLevel="1">
+    <row r="25" spans="1:4" hidden="1" outlineLevel="1">
       <c r="A25" s="4" t="s">
         <v>141</v>
       </c>
@@ -3974,7 +3962,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="26" spans="1:4" outlineLevel="1">
+    <row r="26" spans="1:4" hidden="1" outlineLevel="1">
       <c r="A26" s="4" t="s">
         <v>143</v>
       </c>
@@ -3982,13 +3970,13 @@
         <v>144</v>
       </c>
       <c r="C26" s="28" t="s">
-        <v>385</v>
+        <v>382</v>
       </c>
       <c r="D26" s="17">
         <v>2</v>
       </c>
     </row>
-    <row r="27" spans="1:4" outlineLevel="1">
+    <row r="27" spans="1:4" hidden="1" outlineLevel="1">
       <c r="A27" s="4" t="s">
         <v>145</v>
       </c>
@@ -4002,7 +3990,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="28" spans="1:4" outlineLevel="1">
+    <row r="28" spans="1:4" hidden="1" outlineLevel="1">
       <c r="A28" s="4" t="s">
         <v>148</v>
       </c>
@@ -4016,7 +4004,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="29" spans="1:4" outlineLevel="1">
+    <row r="29" spans="1:4" hidden="1" outlineLevel="1">
       <c r="A29" s="4" t="s">
         <v>149</v>
       </c>
@@ -4030,7 +4018,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="30" spans="1:4" outlineLevel="1">
+    <row r="30" spans="1:4" hidden="1" outlineLevel="1">
       <c r="A30" s="13" t="s">
         <v>151</v>
       </c>
@@ -4044,7 +4032,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="31" spans="1:4" outlineLevel="1">
+    <row r="31" spans="1:4" hidden="1" outlineLevel="1">
       <c r="A31" s="13" t="s">
         <v>154</v>
       </c>
@@ -4052,13 +4040,13 @@
         <v>153</v>
       </c>
       <c r="C31" s="28" t="s">
-        <v>385</v>
+        <v>382</v>
       </c>
       <c r="D31" s="17">
         <v>2</v>
       </c>
     </row>
-    <row r="32" spans="1:4" outlineLevel="1">
+    <row r="32" spans="1:4" hidden="1" outlineLevel="1">
       <c r="A32" s="7" t="s">
         <v>155</v>
       </c>
@@ -4066,13 +4054,13 @@
         <v>156</v>
       </c>
       <c r="C32" s="28" t="s">
-        <v>385</v>
+        <v>382</v>
       </c>
       <c r="D32" s="14">
         <v>3</v>
       </c>
     </row>
-    <row r="33" spans="1:4" outlineLevel="1">
+    <row r="33" spans="1:4" hidden="1" outlineLevel="1">
       <c r="A33" s="4" t="s">
         <v>157</v>
       </c>
@@ -4080,13 +4068,13 @@
         <v>158</v>
       </c>
       <c r="C33" s="28" t="s">
-        <v>385</v>
+        <v>382</v>
       </c>
       <c r="D33" s="14">
         <v>3</v>
       </c>
     </row>
-    <row r="34" spans="1:4" outlineLevel="1">
+    <row r="34" spans="1:4" hidden="1" outlineLevel="1">
       <c r="A34" s="4" t="s">
         <v>159</v>
       </c>
@@ -4094,13 +4082,13 @@
         <v>160</v>
       </c>
       <c r="C34" s="28" t="s">
-        <v>385</v>
+        <v>382</v>
       </c>
       <c r="D34" s="14">
         <v>3</v>
       </c>
     </row>
-    <row r="35" spans="1:4" s="8" customFormat="1" outlineLevel="1" collapsed="1">
+    <row r="35" spans="1:4" s="8" customFormat="1" hidden="1" outlineLevel="1" collapsed="1">
       <c r="A35" s="4" t="s">
         <v>161</v>
       </c>
@@ -4108,13 +4096,13 @@
         <v>162</v>
       </c>
       <c r="C35" s="28" t="s">
-        <v>385</v>
+        <v>382</v>
       </c>
       <c r="D35" s="14">
         <v>3</v>
       </c>
     </row>
-    <row r="36" spans="1:4" outlineLevel="1">
+    <row r="36" spans="1:4" hidden="1" outlineLevel="1">
       <c r="A36" s="13" t="s">
         <v>163</v>
       </c>
@@ -4122,13 +4110,13 @@
         <v>164</v>
       </c>
       <c r="C36" s="28" t="s">
-        <v>385</v>
+        <v>382</v>
       </c>
       <c r="D36" s="14">
         <v>3</v>
       </c>
     </row>
-    <row r="37" spans="1:4" s="8" customFormat="1" outlineLevel="1" collapsed="1">
+    <row r="37" spans="1:4" s="8" customFormat="1" hidden="1" outlineLevel="1" collapsed="1">
       <c r="A37" s="4" t="s">
         <v>165</v>
       </c>
@@ -4136,13 +4124,13 @@
         <v>166</v>
       </c>
       <c r="C37" s="28" t="s">
-        <v>385</v>
+        <v>382</v>
       </c>
       <c r="D37" s="14">
         <v>3</v>
       </c>
     </row>
-    <row r="38" spans="1:4" outlineLevel="1">
+    <row r="38" spans="1:4" hidden="1" outlineLevel="1">
       <c r="A38" s="13" t="s">
         <v>167</v>
       </c>
@@ -4150,13 +4138,13 @@
         <v>168</v>
       </c>
       <c r="C38" s="28" t="s">
-        <v>385</v>
+        <v>382</v>
       </c>
       <c r="D38" s="14">
         <v>3</v>
       </c>
     </row>
-    <row r="39" spans="1:4" outlineLevel="1">
+    <row r="39" spans="1:4" hidden="1" outlineLevel="1">
       <c r="A39" s="13" t="s">
         <v>169</v>
       </c>
@@ -4164,13 +4152,13 @@
         <v>170</v>
       </c>
       <c r="C39" s="28" t="s">
-        <v>385</v>
+        <v>382</v>
       </c>
       <c r="D39" s="14">
         <v>3</v>
       </c>
     </row>
-    <row r="40" spans="1:4" outlineLevel="1">
+    <row r="40" spans="1:4" hidden="1" outlineLevel="1">
       <c r="A40" s="13" t="s">
         <v>171</v>
       </c>
@@ -4184,7 +4172,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="41" spans="1:4" outlineLevel="1">
+    <row r="41" spans="1:4" hidden="1" outlineLevel="1">
       <c r="A41" s="13" t="s">
         <v>173</v>
       </c>
@@ -4198,7 +4186,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="42" spans="1:4" outlineLevel="1">
+    <row r="42" spans="1:4" hidden="1" outlineLevel="1">
       <c r="A42" s="13" t="s">
         <v>175</v>
       </c>
@@ -4212,7 +4200,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="43" spans="1:4" outlineLevel="1">
+    <row r="43" spans="1:4" hidden="1" outlineLevel="1">
       <c r="A43" s="13" t="s">
         <v>177</v>
       </c>
@@ -4226,7 +4214,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="44" spans="1:4" outlineLevel="1">
+    <row r="44" spans="1:4" hidden="1" outlineLevel="1">
       <c r="A44" s="13" t="s">
         <v>179</v>
       </c>
@@ -4240,7 +4228,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="45" spans="1:4" outlineLevel="1">
+    <row r="45" spans="1:4" hidden="1" outlineLevel="1">
       <c r="A45" s="13" t="s">
         <v>181</v>
       </c>
@@ -4254,7 +4242,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="46" spans="1:4" outlineLevel="1">
+    <row r="46" spans="1:4" hidden="1" outlineLevel="1">
       <c r="A46" s="13" t="s">
         <v>183</v>
       </c>
@@ -4268,12 +4256,12 @@
         <v>1</v>
       </c>
     </row>
-    <row r="47" spans="1:4" outlineLevel="1">
+    <row r="47" spans="1:4" hidden="1" outlineLevel="1">
       <c r="A47" s="13" t="s">
         <v>185</v>
       </c>
       <c r="B47" s="11" t="s">
-        <v>343</v>
+        <v>342</v>
       </c>
       <c r="C47" s="10" t="s">
         <v>3</v>
@@ -4282,12 +4270,12 @@
         <v>1</v>
       </c>
     </row>
-    <row r="48" spans="1:4" outlineLevel="1">
+    <row r="48" spans="1:4" hidden="1" outlineLevel="1">
       <c r="A48" s="13" t="s">
         <v>186</v>
       </c>
       <c r="B48" s="9" t="s">
-        <v>344</v>
+        <v>343</v>
       </c>
       <c r="C48" s="10" t="s">
         <v>3</v>
@@ -4296,7 +4284,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="49" spans="1:4" outlineLevel="1">
+    <row r="49" spans="1:4" hidden="1" outlineLevel="1">
       <c r="A49" s="13" t="s">
         <v>187</v>
       </c>
@@ -4310,7 +4298,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="50" spans="1:4" outlineLevel="1">
+    <row r="50" spans="1:4" hidden="1" outlineLevel="1">
       <c r="A50" s="13" t="s">
         <v>189</v>
       </c>
@@ -4318,13 +4306,13 @@
         <v>190</v>
       </c>
       <c r="C50" s="28" t="s">
-        <v>385</v>
+        <v>382</v>
       </c>
       <c r="D50" s="17">
         <v>2</v>
       </c>
     </row>
-    <row r="51" spans="1:4" s="8" customFormat="1" outlineLevel="1" collapsed="1">
+    <row r="51" spans="1:4" s="8" customFormat="1" hidden="1" outlineLevel="1" collapsed="1">
       <c r="A51" s="13" t="s">
         <v>191</v>
       </c>
@@ -4332,13 +4320,13 @@
         <v>192</v>
       </c>
       <c r="C51" s="28" t="s">
-        <v>385</v>
+        <v>382</v>
       </c>
       <c r="D51" s="17">
         <v>2</v>
       </c>
     </row>
-    <row r="52" spans="1:4" outlineLevel="1">
+    <row r="52" spans="1:4" hidden="1" outlineLevel="1">
       <c r="A52" s="13" t="s">
         <v>193</v>
       </c>
@@ -4346,13 +4334,13 @@
         <v>194</v>
       </c>
       <c r="C52" s="28" t="s">
-        <v>385</v>
+        <v>382</v>
       </c>
       <c r="D52" s="17">
         <v>2</v>
       </c>
     </row>
-    <row r="53" spans="1:4" s="8" customFormat="1" outlineLevel="1" collapsed="1">
+    <row r="53" spans="1:4" s="8" customFormat="1" hidden="1" outlineLevel="1" collapsed="1">
       <c r="A53" s="4" t="s">
         <v>195</v>
       </c>
@@ -4360,13 +4348,13 @@
         <v>196</v>
       </c>
       <c r="C53" s="28" t="s">
-        <v>385</v>
+        <v>382</v>
       </c>
       <c r="D53" s="14">
         <v>2</v>
       </c>
     </row>
-    <row r="54" spans="1:4" outlineLevel="1">
+    <row r="54" spans="1:4" hidden="1" outlineLevel="1">
       <c r="A54" s="13" t="s">
         <v>197</v>
       </c>
@@ -4374,13 +4362,13 @@
         <v>198</v>
       </c>
       <c r="C54" s="28" t="s">
-        <v>385</v>
+        <v>382</v>
       </c>
       <c r="D54" s="17">
         <v>2</v>
       </c>
     </row>
-    <row r="55" spans="1:4" outlineLevel="1">
+    <row r="55" spans="1:4" hidden="1" outlineLevel="1">
       <c r="A55" s="13" t="s">
         <v>199</v>
       </c>
@@ -4388,13 +4376,13 @@
         <v>200</v>
       </c>
       <c r="C55" s="28" t="s">
-        <v>385</v>
+        <v>382</v>
       </c>
       <c r="D55" s="17">
         <v>2</v>
       </c>
     </row>
-    <row r="56" spans="1:4">
+    <row r="56" spans="1:4" collapsed="1">
       <c r="A56" s="21" t="s">
         <v>121</v>
       </c>
@@ -4403,10 +4391,10 @@
       </c>
       <c r="C56" s="23"/>
       <c r="D56" s="24" t="s">
-        <v>379</v>
-      </c>
-    </row>
-    <row r="57" spans="1:4" outlineLevel="1">
+        <v>376</v>
+      </c>
+    </row>
+    <row r="57" spans="1:4" hidden="1" outlineLevel="1">
       <c r="A57" s="4" t="s">
         <v>5</v>
       </c>
@@ -4420,7 +4408,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="58" spans="1:4" outlineLevel="1">
+    <row r="58" spans="1:4" hidden="1" outlineLevel="1">
       <c r="A58" s="4" t="s">
         <v>6</v>
       </c>
@@ -4428,13 +4416,13 @@
         <v>8</v>
       </c>
       <c r="C58" s="3" t="s">
-        <v>385</v>
+        <v>382</v>
       </c>
       <c r="D58" s="14">
         <v>2</v>
       </c>
     </row>
-    <row r="59" spans="1:4" s="8" customFormat="1" outlineLevel="1" collapsed="1">
+    <row r="59" spans="1:4" s="8" customFormat="1" hidden="1" outlineLevel="1" collapsed="1">
       <c r="A59" s="4" t="s">
         <v>10</v>
       </c>
@@ -4442,13 +4430,13 @@
         <v>11</v>
       </c>
       <c r="C59" s="3" t="s">
-        <v>385</v>
+        <v>382</v>
       </c>
       <c r="D59" s="14">
         <v>3</v>
       </c>
     </row>
-    <row r="60" spans="1:4" outlineLevel="1">
+    <row r="60" spans="1:4" hidden="1" outlineLevel="1">
       <c r="A60" s="4" t="s">
         <v>13</v>
       </c>
@@ -4456,13 +4444,13 @@
         <v>12</v>
       </c>
       <c r="C60" s="3" t="s">
-        <v>385</v>
+        <v>382</v>
       </c>
       <c r="D60" s="14">
         <v>3</v>
       </c>
     </row>
-    <row r="61" spans="1:4" s="8" customFormat="1" outlineLevel="1" collapsed="1">
+    <row r="61" spans="1:4" s="8" customFormat="1" hidden="1" outlineLevel="1" collapsed="1">
       <c r="A61" s="4" t="s">
         <v>14</v>
       </c>
@@ -4476,7 +4464,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="62" spans="1:4" outlineLevel="1">
+    <row r="62" spans="1:4" hidden="1" outlineLevel="1">
       <c r="A62" s="4" t="s">
         <v>17</v>
       </c>
@@ -4484,13 +4472,13 @@
         <v>18</v>
       </c>
       <c r="C62" s="28" t="s">
-        <v>385</v>
+        <v>382</v>
       </c>
       <c r="D62" s="14">
         <v>3</v>
       </c>
     </row>
-    <row r="63" spans="1:4" s="8" customFormat="1" outlineLevel="1" collapsed="1">
+    <row r="63" spans="1:4" s="8" customFormat="1" hidden="1" outlineLevel="1" collapsed="1">
       <c r="A63" s="4" t="s">
         <v>16</v>
       </c>
@@ -4498,13 +4486,13 @@
         <v>19</v>
       </c>
       <c r="C63" s="28" t="s">
-        <v>385</v>
+        <v>382</v>
       </c>
       <c r="D63" s="14">
         <v>3</v>
       </c>
     </row>
-    <row r="64" spans="1:4" outlineLevel="1">
+    <row r="64" spans="1:4" hidden="1" outlineLevel="1">
       <c r="A64" s="4" t="s">
         <v>22</v>
       </c>
@@ -4512,13 +4500,13 @@
         <v>21</v>
       </c>
       <c r="C64" s="28" t="s">
-        <v>385</v>
+        <v>382</v>
       </c>
       <c r="D64" s="14">
         <v>3</v>
       </c>
     </row>
-    <row r="65" spans="1:4" s="8" customFormat="1" outlineLevel="1" collapsed="1">
+    <row r="65" spans="1:4" s="8" customFormat="1" hidden="1" outlineLevel="1" collapsed="1">
       <c r="A65" s="4" t="s">
         <v>23</v>
       </c>
@@ -4526,13 +4514,13 @@
         <v>25</v>
       </c>
       <c r="C65" s="28" t="s">
-        <v>385</v>
+        <v>382</v>
       </c>
       <c r="D65" s="14">
         <v>3</v>
       </c>
     </row>
-    <row r="66" spans="1:4" outlineLevel="1">
+    <row r="66" spans="1:4" hidden="1" outlineLevel="1">
       <c r="A66" s="4" t="s">
         <v>24</v>
       </c>
@@ -4540,13 +4528,13 @@
         <v>26</v>
       </c>
       <c r="C66" s="28" t="s">
-        <v>385</v>
+        <v>382</v>
       </c>
       <c r="D66" s="14">
         <v>3</v>
       </c>
     </row>
-    <row r="67" spans="1:4" s="8" customFormat="1" outlineLevel="1" collapsed="1">
+    <row r="67" spans="1:4" s="8" customFormat="1" hidden="1" outlineLevel="1" collapsed="1">
       <c r="A67" s="4" t="s">
         <v>20</v>
       </c>
@@ -4554,13 +4542,13 @@
         <v>27</v>
       </c>
       <c r="C67" s="28" t="s">
-        <v>385</v>
+        <v>382</v>
       </c>
       <c r="D67" s="14">
         <v>3</v>
       </c>
     </row>
-    <row r="68" spans="1:4" outlineLevel="1">
+    <row r="68" spans="1:4" hidden="1" outlineLevel="1">
       <c r="A68" s="4" t="s">
         <v>28</v>
       </c>
@@ -4568,13 +4556,13 @@
         <v>29</v>
       </c>
       <c r="C68" s="28" t="s">
-        <v>385</v>
+        <v>382</v>
       </c>
       <c r="D68" s="14">
         <v>3</v>
       </c>
     </row>
-    <row r="69" spans="1:4" outlineLevel="1">
+    <row r="69" spans="1:4" hidden="1" outlineLevel="1">
       <c r="A69" s="4" t="s">
         <v>30</v>
       </c>
@@ -4582,13 +4570,13 @@
         <v>31</v>
       </c>
       <c r="C69" s="28" t="s">
-        <v>385</v>
+        <v>382</v>
       </c>
       <c r="D69" s="14">
         <v>4</v>
       </c>
     </row>
-    <row r="70" spans="1:4" outlineLevel="1">
+    <row r="70" spans="1:4" hidden="1" outlineLevel="1">
       <c r="A70" s="4" t="s">
         <v>32</v>
       </c>
@@ -4596,13 +4584,13 @@
         <v>35</v>
       </c>
       <c r="C70" s="28" t="s">
-        <v>385</v>
+        <v>382</v>
       </c>
       <c r="D70" s="14">
         <v>3</v>
       </c>
     </row>
-    <row r="71" spans="1:4" outlineLevel="1">
+    <row r="71" spans="1:4" hidden="1" outlineLevel="1">
       <c r="A71" s="4" t="s">
         <v>33</v>
       </c>
@@ -4610,13 +4598,13 @@
         <v>34</v>
       </c>
       <c r="C71" s="28" t="s">
-        <v>385</v>
+        <v>382</v>
       </c>
       <c r="D71" s="14">
         <v>3</v>
       </c>
     </row>
-    <row r="72" spans="1:4" outlineLevel="1">
+    <row r="72" spans="1:4" hidden="1" outlineLevel="1">
       <c r="A72" s="4" t="s">
         <v>36</v>
       </c>
@@ -4624,13 +4612,13 @@
         <v>39</v>
       </c>
       <c r="C72" s="28" t="s">
-        <v>385</v>
+        <v>382</v>
       </c>
       <c r="D72" s="14">
         <v>3</v>
       </c>
     </row>
-    <row r="73" spans="1:4" outlineLevel="1">
+    <row r="73" spans="1:4" hidden="1" outlineLevel="1">
       <c r="A73" s="4" t="s">
         <v>37</v>
       </c>
@@ -4638,13 +4626,13 @@
         <v>40</v>
       </c>
       <c r="C73" s="28" t="s">
-        <v>385</v>
+        <v>382</v>
       </c>
       <c r="D73" s="14">
         <v>3</v>
       </c>
     </row>
-    <row r="74" spans="1:4" outlineLevel="1">
+    <row r="74" spans="1:4" hidden="1" outlineLevel="1">
       <c r="A74" s="4" t="s">
         <v>38</v>
       </c>
@@ -4652,13 +4640,13 @@
         <v>41</v>
       </c>
       <c r="C74" s="28" t="s">
-        <v>385</v>
+        <v>382</v>
       </c>
       <c r="D74" s="14">
         <v>3</v>
       </c>
     </row>
-    <row r="75" spans="1:4" outlineLevel="1">
+    <row r="75" spans="1:4" hidden="1" outlineLevel="1">
       <c r="A75" s="4" t="s">
         <v>42</v>
       </c>
@@ -4672,7 +4660,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="76" spans="1:4" outlineLevel="1">
+    <row r="76" spans="1:4" hidden="1" outlineLevel="1">
       <c r="A76" s="4" t="s">
         <v>44</v>
       </c>
@@ -4686,7 +4674,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="77" spans="1:4" outlineLevel="1">
+    <row r="77" spans="1:4" hidden="1" outlineLevel="1">
       <c r="A77" s="4" t="s">
         <v>46</v>
       </c>
@@ -4700,12 +4688,12 @@
         <v>1</v>
       </c>
     </row>
-    <row r="78" spans="1:4" outlineLevel="1">
+    <row r="78" spans="1:4" hidden="1" outlineLevel="1">
       <c r="A78" s="4" t="s">
-        <v>375</v>
+        <v>372</v>
       </c>
       <c r="B78" s="2" t="s">
-        <v>376</v>
+        <v>373</v>
       </c>
       <c r="C78" s="3" t="s">
         <v>3</v>
@@ -4714,12 +4702,12 @@
         <v>1</v>
       </c>
     </row>
-    <row r="79" spans="1:4" outlineLevel="1">
+    <row r="79" spans="1:4" hidden="1" outlineLevel="1">
       <c r="A79" s="4" t="s">
-        <v>393</v>
+        <v>390</v>
       </c>
       <c r="B79" s="2" t="s">
-        <v>394</v>
+        <v>391</v>
       </c>
       <c r="C79" s="3" t="s">
         <v>3</v>
@@ -4728,7 +4716,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="80" spans="1:4">
+    <row r="80" spans="1:4" collapsed="1">
       <c r="A80" s="21" t="s">
         <v>0</v>
       </c>
@@ -4737,10 +4725,10 @@
       </c>
       <c r="C80" s="23"/>
       <c r="D80" s="24" t="s">
-        <v>379</v>
-      </c>
-    </row>
-    <row r="81" spans="1:4" outlineLevel="1">
+        <v>376</v>
+      </c>
+    </row>
+    <row r="81" spans="1:4" hidden="1" outlineLevel="1">
       <c r="A81" s="4" t="s">
         <v>104</v>
       </c>
@@ -4754,7 +4742,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="82" spans="1:4" outlineLevel="1">
+    <row r="82" spans="1:4" hidden="1" outlineLevel="1">
       <c r="A82" s="13" t="s">
         <v>105</v>
       </c>
@@ -4768,7 +4756,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="83" spans="1:4" outlineLevel="1">
+    <row r="83" spans="1:4" hidden="1" outlineLevel="1">
       <c r="A83" s="13" t="s">
         <v>107</v>
       </c>
@@ -4782,7 +4770,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="84" spans="1:4" outlineLevel="1">
+    <row r="84" spans="1:4" hidden="1" outlineLevel="1">
       <c r="A84" s="4" t="s">
         <v>109</v>
       </c>
@@ -4796,7 +4784,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="85" spans="1:4" outlineLevel="1">
+    <row r="85" spans="1:4" hidden="1" outlineLevel="1">
       <c r="A85" s="4" t="s">
         <v>111</v>
       </c>
@@ -4810,7 +4798,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="86" spans="1:4">
+    <row r="86" spans="1:4" collapsed="1">
       <c r="A86" s="21" t="s">
         <v>101</v>
       </c>
@@ -4819,953 +4807,953 @@
       </c>
       <c r="C86" s="23"/>
       <c r="D86" s="24" t="s">
-        <v>379</v>
-      </c>
-    </row>
-    <row r="87" spans="1:4" outlineLevel="1">
+        <v>376</v>
+      </c>
+    </row>
+    <row r="87" spans="1:4" hidden="1" outlineLevel="1">
       <c r="A87" s="4" t="s">
+        <v>337</v>
+      </c>
+      <c r="B87" s="15" t="s">
         <v>338</v>
       </c>
-      <c r="B87" s="15" t="s">
+      <c r="C87" s="28" t="s">
+        <v>382</v>
+      </c>
+      <c r="D87" s="14">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="88" spans="1:4" hidden="1" outlineLevel="1">
+      <c r="A88" s="4" t="s">
         <v>339</v>
       </c>
-      <c r="C87" s="28" t="s">
-        <v>385</v>
-      </c>
-      <c r="D87" s="14">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="88" spans="1:4" outlineLevel="1">
-      <c r="A88" s="4" t="s">
+      <c r="B88" s="15" t="s">
         <v>340</v>
       </c>
-      <c r="B88" s="15" t="s">
-        <v>341</v>
-      </c>
       <c r="C88" s="28" t="s">
-        <v>385</v>
+        <v>382</v>
       </c>
       <c r="D88" s="14">
         <v>3</v>
       </c>
     </row>
-    <row r="89" spans="1:4" outlineLevel="1">
+    <row r="89" spans="1:4" hidden="1" outlineLevel="1">
       <c r="A89" s="4" t="s">
+        <v>331</v>
+      </c>
+      <c r="B89" s="15" t="s">
         <v>332</v>
       </c>
-      <c r="B89" s="15" t="s">
+      <c r="C89" s="28" t="s">
+        <v>382</v>
+      </c>
+      <c r="D89" s="14">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="90" spans="1:4" hidden="1" outlineLevel="1">
+      <c r="A90" s="4" t="s">
         <v>333</v>
       </c>
-      <c r="C89" s="28" t="s">
-        <v>385</v>
-      </c>
-      <c r="D89" s="14">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="90" spans="1:4" outlineLevel="1">
-      <c r="A90" s="4" t="s">
+      <c r="B90" s="15" t="s">
         <v>334</v>
       </c>
-      <c r="B90" s="15" t="s">
+      <c r="C90" s="28" t="s">
+        <v>382</v>
+      </c>
+      <c r="D90" s="14">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="91" spans="1:4" hidden="1" outlineLevel="1">
+      <c r="A91" s="4" t="s">
         <v>335</v>
       </c>
-      <c r="C90" s="28" t="s">
-        <v>385</v>
-      </c>
-      <c r="D90" s="14">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="91" spans="1:4" outlineLevel="1">
-      <c r="A91" s="4" t="s">
+      <c r="B91" s="15" t="s">
         <v>336</v>
       </c>
-      <c r="B91" s="15" t="s">
-        <v>337</v>
-      </c>
       <c r="C91" s="28" t="s">
-        <v>385</v>
+        <v>382</v>
       </c>
       <c r="D91" s="14">
         <v>3</v>
       </c>
     </row>
-    <row r="92" spans="1:4" outlineLevel="1" collapsed="1">
+    <row r="92" spans="1:4" hidden="1" outlineLevel="1" collapsed="1">
       <c r="A92" s="4" t="s">
+        <v>329</v>
+      </c>
+      <c r="B92" s="15" t="s">
         <v>330</v>
       </c>
-      <c r="B92" s="15" t="s">
-        <v>331</v>
-      </c>
       <c r="C92" s="28" t="s">
-        <v>385</v>
+        <v>382</v>
       </c>
       <c r="D92" s="14">
         <v>3</v>
       </c>
     </row>
-    <row r="93" spans="1:4" outlineLevel="1">
+    <row r="93" spans="1:4" hidden="1" outlineLevel="1">
       <c r="A93" s="4" t="s">
+        <v>327</v>
+      </c>
+      <c r="B93" s="15" t="s">
         <v>328</v>
       </c>
-      <c r="B93" s="15" t="s">
-        <v>329</v>
-      </c>
       <c r="C93" s="28" t="s">
-        <v>385</v>
+        <v>382</v>
       </c>
       <c r="D93" s="14">
         <v>3</v>
       </c>
     </row>
-    <row r="94" spans="1:4" outlineLevel="1">
+    <row r="94" spans="1:4" hidden="1" outlineLevel="1">
       <c r="A94" s="4" t="s">
+        <v>323</v>
+      </c>
+      <c r="B94" s="15" t="s">
         <v>324</v>
       </c>
-      <c r="B94" s="15" t="s">
+      <c r="C94" s="28" t="s">
+        <v>382</v>
+      </c>
+      <c r="D94" s="14">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="95" spans="1:4" hidden="1" outlineLevel="1">
+      <c r="A95" s="4" t="s">
         <v>325</v>
       </c>
-      <c r="C94" s="28" t="s">
-        <v>385</v>
-      </c>
-      <c r="D94" s="14">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="95" spans="1:4" outlineLevel="1">
-      <c r="A95" s="4" t="s">
+      <c r="B95" s="15" t="s">
         <v>326</v>
       </c>
-      <c r="B95" s="15" t="s">
-        <v>327</v>
-      </c>
       <c r="C95" s="28" t="s">
-        <v>385</v>
+        <v>382</v>
       </c>
       <c r="D95" s="14">
         <v>3</v>
       </c>
     </row>
-    <row r="96" spans="1:4" outlineLevel="1">
+    <row r="96" spans="1:4" hidden="1" outlineLevel="1">
       <c r="A96" s="4" t="s">
+        <v>317</v>
+      </c>
+      <c r="B96" s="15" t="s">
         <v>318</v>
       </c>
-      <c r="B96" s="15" t="s">
+      <c r="C96" s="28" t="s">
+        <v>382</v>
+      </c>
+      <c r="D96" s="14">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="97" spans="1:4" hidden="1" outlineLevel="1">
+      <c r="A97" s="4" t="s">
         <v>319</v>
       </c>
-      <c r="C96" s="28" t="s">
-        <v>385</v>
-      </c>
-      <c r="D96" s="14">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="97" spans="1:4" outlineLevel="1">
-      <c r="A97" s="4" t="s">
+      <c r="B97" s="15" t="s">
         <v>320</v>
       </c>
-      <c r="B97" s="15" t="s">
+      <c r="C97" s="28" t="s">
+        <v>382</v>
+      </c>
+      <c r="D97" s="14">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="98" spans="1:4" hidden="1" outlineLevel="1" collapsed="1">
+      <c r="A98" s="4" t="s">
         <v>321</v>
       </c>
-      <c r="C97" s="28" t="s">
-        <v>385</v>
-      </c>
-      <c r="D97" s="14">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="98" spans="1:4" outlineLevel="1" collapsed="1">
-      <c r="A98" s="4" t="s">
+      <c r="B98" s="15" t="s">
         <v>322</v>
       </c>
-      <c r="B98" s="15" t="s">
-        <v>323</v>
-      </c>
       <c r="C98" s="28" t="s">
-        <v>385</v>
+        <v>382</v>
       </c>
       <c r="D98" s="14">
         <v>3</v>
       </c>
     </row>
-    <row r="99" spans="1:4" outlineLevel="1">
+    <row r="99" spans="1:4" hidden="1" outlineLevel="1">
       <c r="A99" s="4" t="s">
+        <v>315</v>
+      </c>
+      <c r="B99" s="15" t="s">
         <v>316</v>
       </c>
-      <c r="B99" s="15" t="s">
-        <v>317</v>
-      </c>
       <c r="C99" s="28" t="s">
-        <v>385</v>
+        <v>382</v>
       </c>
       <c r="D99" s="14">
         <v>3</v>
       </c>
     </row>
-    <row r="100" spans="1:4" outlineLevel="1">
+    <row r="100" spans="1:4" hidden="1" outlineLevel="1">
       <c r="A100" s="4" t="s">
+        <v>311</v>
+      </c>
+      <c r="B100" s="15" t="s">
         <v>312</v>
       </c>
-      <c r="B100" s="15" t="s">
+      <c r="C100" s="28" t="s">
+        <v>382</v>
+      </c>
+      <c r="D100" s="14">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="101" spans="1:4" hidden="1" outlineLevel="1">
+      <c r="A101" s="4" t="s">
         <v>313</v>
       </c>
-      <c r="C100" s="28" t="s">
-        <v>385</v>
-      </c>
-      <c r="D100" s="14">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="101" spans="1:4" outlineLevel="1">
-      <c r="A101" s="4" t="s">
+      <c r="B101" s="15" t="s">
         <v>314</v>
       </c>
-      <c r="B101" s="15" t="s">
-        <v>315</v>
-      </c>
       <c r="C101" s="28" t="s">
-        <v>385</v>
+        <v>382</v>
       </c>
       <c r="D101" s="14">
         <v>3</v>
       </c>
     </row>
-    <row r="102" spans="1:4" outlineLevel="1">
+    <row r="102" spans="1:4" hidden="1" outlineLevel="1">
       <c r="A102" s="4" t="s">
+        <v>309</v>
+      </c>
+      <c r="B102" s="15" t="s">
         <v>310</v>
       </c>
-      <c r="B102" s="15" t="s">
-        <v>311</v>
-      </c>
       <c r="C102" s="28" t="s">
-        <v>385</v>
+        <v>382</v>
       </c>
       <c r="D102" s="14">
         <v>3</v>
       </c>
     </row>
-    <row r="103" spans="1:4" outlineLevel="1">
+    <row r="103" spans="1:4" hidden="1" outlineLevel="1">
       <c r="A103" s="4" t="s">
+        <v>307</v>
+      </c>
+      <c r="B103" s="15" t="s">
         <v>308</v>
       </c>
-      <c r="B103" s="15" t="s">
-        <v>309</v>
-      </c>
       <c r="C103" s="28" t="s">
-        <v>385</v>
+        <v>382</v>
       </c>
       <c r="D103" s="14">
         <v>3</v>
       </c>
     </row>
-    <row r="104" spans="1:4" outlineLevel="1">
+    <row r="104" spans="1:4" hidden="1" outlineLevel="1">
       <c r="A104" s="4" t="s">
+        <v>305</v>
+      </c>
+      <c r="B104" s="15" t="s">
         <v>306</v>
       </c>
-      <c r="B104" s="15" t="s">
+      <c r="C104" s="28" t="s">
+        <v>382</v>
+      </c>
+      <c r="D104" s="14">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="105" spans="1:4" hidden="1" outlineLevel="1">
+      <c r="A105" s="4" t="s">
         <v>307</v>
       </c>
-      <c r="C104" s="28" t="s">
-        <v>385</v>
-      </c>
-      <c r="D104" s="14">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="105" spans="1:4" outlineLevel="1">
-      <c r="A105" s="4" t="s">
+      <c r="B105" s="15" t="s">
         <v>308</v>
       </c>
-      <c r="B105" s="15" t="s">
-        <v>309</v>
-      </c>
       <c r="C105" s="28" t="s">
-        <v>385</v>
+        <v>382</v>
       </c>
       <c r="D105" s="14">
         <v>3</v>
       </c>
     </row>
-    <row r="106" spans="1:4" outlineLevel="1">
+    <row r="106" spans="1:4" hidden="1" outlineLevel="1">
       <c r="A106" s="4" t="s">
+        <v>299</v>
+      </c>
+      <c r="B106" s="15" t="s">
         <v>300</v>
       </c>
-      <c r="B106" s="15" t="s">
+      <c r="C106" s="28" t="s">
+        <v>382</v>
+      </c>
+      <c r="D106" s="14">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="107" spans="1:4" hidden="1" outlineLevel="1">
+      <c r="A107" s="4" t="s">
         <v>301</v>
       </c>
-      <c r="C106" s="28" t="s">
-        <v>385</v>
-      </c>
-      <c r="D106" s="14">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="107" spans="1:4" outlineLevel="1">
-      <c r="A107" s="4" t="s">
+      <c r="B107" s="15" t="s">
         <v>302</v>
       </c>
-      <c r="B107" s="15" t="s">
+      <c r="C107" s="28" t="s">
+        <v>382</v>
+      </c>
+      <c r="D107" s="14">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="108" spans="1:4" hidden="1" outlineLevel="1">
+      <c r="A108" s="4" t="s">
         <v>303</v>
       </c>
-      <c r="C107" s="28" t="s">
-        <v>385</v>
-      </c>
-      <c r="D107" s="14">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="108" spans="1:4" outlineLevel="1">
-      <c r="A108" s="4" t="s">
+      <c r="B108" s="15" t="s">
         <v>304</v>
       </c>
-      <c r="B108" s="15" t="s">
-        <v>305</v>
-      </c>
       <c r="C108" s="28" t="s">
-        <v>385</v>
+        <v>382</v>
       </c>
       <c r="D108" s="14">
         <v>3</v>
       </c>
     </row>
-    <row r="109" spans="1:4" outlineLevel="1">
+    <row r="109" spans="1:4" hidden="1" outlineLevel="1">
       <c r="A109" s="4" t="s">
+        <v>295</v>
+      </c>
+      <c r="B109" s="15" t="s">
         <v>296</v>
       </c>
-      <c r="B109" s="15" t="s">
+      <c r="C109" s="28" t="s">
+        <v>382</v>
+      </c>
+      <c r="D109" s="14">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="110" spans="1:4" hidden="1" outlineLevel="1">
+      <c r="A110" s="4" t="s">
         <v>297</v>
       </c>
-      <c r="C109" s="28" t="s">
-        <v>385</v>
-      </c>
-      <c r="D109" s="14">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="110" spans="1:4" outlineLevel="1">
-      <c r="A110" s="4" t="s">
+      <c r="B110" s="15" t="s">
         <v>298</v>
       </c>
-      <c r="B110" s="15" t="s">
-        <v>299</v>
-      </c>
       <c r="C110" s="28" t="s">
-        <v>385</v>
+        <v>382</v>
       </c>
       <c r="D110" s="14">
         <v>3</v>
       </c>
     </row>
-    <row r="111" spans="1:4" outlineLevel="1">
+    <row r="111" spans="1:4" hidden="1" outlineLevel="1">
       <c r="A111" s="4" t="s">
+        <v>293</v>
+      </c>
+      <c r="B111" s="15" t="s">
         <v>294</v>
       </c>
-      <c r="B111" s="15" t="s">
-        <v>295</v>
-      </c>
       <c r="C111" s="28" t="s">
-        <v>385</v>
+        <v>382</v>
       </c>
       <c r="D111" s="14">
         <v>3</v>
       </c>
     </row>
-    <row r="112" spans="1:4" outlineLevel="1">
+    <row r="112" spans="1:4" hidden="1" outlineLevel="1">
       <c r="A112" s="4" t="s">
+        <v>287</v>
+      </c>
+      <c r="B112" s="15" t="s">
         <v>288</v>
       </c>
-      <c r="B112" s="15" t="s">
+      <c r="C112" s="28" t="s">
+        <v>382</v>
+      </c>
+      <c r="D112" s="14">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="113" spans="1:4" hidden="1" outlineLevel="1">
+      <c r="A113" s="4" t="s">
         <v>289</v>
       </c>
-      <c r="C112" s="28" t="s">
-        <v>385</v>
-      </c>
-      <c r="D112" s="14">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="113" spans="1:4" outlineLevel="1">
-      <c r="A113" s="4" t="s">
+      <c r="B113" s="15" t="s">
         <v>290</v>
       </c>
-      <c r="B113" s="15" t="s">
+      <c r="C113" s="28" t="s">
+        <v>382</v>
+      </c>
+      <c r="D113" s="14">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="114" spans="1:4" hidden="1" outlineLevel="1">
+      <c r="A114" s="4" t="s">
         <v>291</v>
       </c>
-      <c r="C113" s="28" t="s">
-        <v>385</v>
-      </c>
-      <c r="D113" s="14">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="114" spans="1:4" outlineLevel="1">
-      <c r="A114" s="4" t="s">
+      <c r="B114" s="15" t="s">
         <v>292</v>
       </c>
-      <c r="B114" s="15" t="s">
-        <v>293</v>
-      </c>
       <c r="C114" s="28" t="s">
-        <v>385</v>
+        <v>382</v>
       </c>
       <c r="D114" s="14">
         <v>3</v>
       </c>
     </row>
-    <row r="115" spans="1:4" outlineLevel="1">
+    <row r="115" spans="1:4" hidden="1" outlineLevel="1">
       <c r="A115" s="4" t="s">
+        <v>283</v>
+      </c>
+      <c r="B115" s="15" t="s">
         <v>284</v>
       </c>
-      <c r="B115" s="15" t="s">
+      <c r="C115" s="28" t="s">
+        <v>382</v>
+      </c>
+      <c r="D115" s="14">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="116" spans="1:4" hidden="1" outlineLevel="1">
+      <c r="A116" s="4" t="s">
         <v>285</v>
       </c>
-      <c r="C115" s="28" t="s">
-        <v>385</v>
-      </c>
-      <c r="D115" s="14">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="116" spans="1:4" outlineLevel="1">
-      <c r="A116" s="4" t="s">
+      <c r="B116" s="15" t="s">
         <v>286</v>
       </c>
-      <c r="B116" s="15" t="s">
-        <v>287</v>
-      </c>
       <c r="C116" s="28" t="s">
-        <v>385</v>
+        <v>382</v>
       </c>
       <c r="D116" s="14">
         <v>3</v>
       </c>
     </row>
-    <row r="117" spans="1:4" outlineLevel="1">
+    <row r="117" spans="1:4" hidden="1" outlineLevel="1">
       <c r="A117" s="4" t="s">
+        <v>277</v>
+      </c>
+      <c r="B117" s="15" t="s">
         <v>278</v>
       </c>
-      <c r="B117" s="15" t="s">
+      <c r="C117" s="28" t="s">
+        <v>382</v>
+      </c>
+      <c r="D117" s="14">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="118" spans="1:4" s="8" customFormat="1" hidden="1" outlineLevel="1">
+      <c r="A118" s="4" t="s">
         <v>279</v>
       </c>
-      <c r="C117" s="28" t="s">
-        <v>385</v>
-      </c>
-      <c r="D117" s="14">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="118" spans="1:4" s="8" customFormat="1" outlineLevel="1">
-      <c r="A118" s="4" t="s">
+      <c r="B118" s="15" t="s">
         <v>280</v>
       </c>
-      <c r="B118" s="15" t="s">
+      <c r="C118" s="28" t="s">
+        <v>382</v>
+      </c>
+      <c r="D118" s="14">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="119" spans="1:4" hidden="1" outlineLevel="1">
+      <c r="A119" s="4" t="s">
         <v>281</v>
       </c>
-      <c r="C118" s="28" t="s">
-        <v>385</v>
-      </c>
-      <c r="D118" s="14">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="119" spans="1:4" outlineLevel="1">
-      <c r="A119" s="4" t="s">
+      <c r="B119" s="15" t="s">
         <v>282</v>
       </c>
-      <c r="B119" s="15" t="s">
-        <v>283</v>
-      </c>
       <c r="C119" s="28" t="s">
-        <v>385</v>
+        <v>382</v>
       </c>
       <c r="D119" s="14">
         <v>3</v>
       </c>
     </row>
-    <row r="120" spans="1:4" outlineLevel="1">
+    <row r="120" spans="1:4" hidden="1" outlineLevel="1">
       <c r="A120" s="4" t="s">
+        <v>275</v>
+      </c>
+      <c r="B120" s="15" t="s">
         <v>276</v>
       </c>
-      <c r="B120" s="15" t="s">
-        <v>277</v>
-      </c>
       <c r="C120" s="28" t="s">
-        <v>385</v>
+        <v>382</v>
       </c>
       <c r="D120" s="14">
         <v>3</v>
       </c>
     </row>
-    <row r="121" spans="1:4" outlineLevel="1">
+    <row r="121" spans="1:4" hidden="1" outlineLevel="1">
       <c r="A121" s="4" t="s">
+        <v>271</v>
+      </c>
+      <c r="B121" s="15" t="s">
         <v>272</v>
       </c>
-      <c r="B121" s="15" t="s">
+      <c r="C121" s="28" t="s">
+        <v>382</v>
+      </c>
+      <c r="D121" s="14">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="122" spans="1:4" hidden="1" outlineLevel="1">
+      <c r="A122" s="4" t="s">
         <v>273</v>
       </c>
-      <c r="C121" s="28" t="s">
-        <v>385</v>
-      </c>
-      <c r="D121" s="14">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="122" spans="1:4" outlineLevel="1">
-      <c r="A122" s="4" t="s">
+      <c r="B122" s="15" t="s">
         <v>274</v>
       </c>
-      <c r="B122" s="15" t="s">
-        <v>275</v>
-      </c>
       <c r="C122" s="28" t="s">
-        <v>385</v>
+        <v>382</v>
       </c>
       <c r="D122" s="14">
         <v>3</v>
       </c>
     </row>
-    <row r="123" spans="1:4" outlineLevel="1">
+    <row r="123" spans="1:4" hidden="1" outlineLevel="1">
       <c r="A123" s="4" t="s">
+        <v>265</v>
+      </c>
+      <c r="B123" s="15" t="s">
         <v>266</v>
       </c>
-      <c r="B123" s="15" t="s">
+      <c r="C123" s="28" t="s">
+        <v>382</v>
+      </c>
+      <c r="D123" s="14">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="124" spans="1:4" hidden="1" outlineLevel="1">
+      <c r="A124" s="4" t="s">
         <v>267</v>
       </c>
-      <c r="C123" s="28" t="s">
-        <v>385</v>
-      </c>
-      <c r="D123" s="14">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="124" spans="1:4" outlineLevel="1">
-      <c r="A124" s="4" t="s">
+      <c r="B124" s="15" t="s">
         <v>268</v>
       </c>
-      <c r="B124" s="15" t="s">
+      <c r="C124" s="28" t="s">
+        <v>382</v>
+      </c>
+      <c r="D124" s="14">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="125" spans="1:4" hidden="1" outlineLevel="1">
+      <c r="A125" s="4" t="s">
         <v>269</v>
       </c>
-      <c r="C124" s="28" t="s">
-        <v>385</v>
-      </c>
-      <c r="D124" s="14">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="125" spans="1:4" outlineLevel="1">
-      <c r="A125" s="4" t="s">
+      <c r="B125" s="15" t="s">
         <v>270</v>
       </c>
-      <c r="B125" s="15" t="s">
-        <v>271</v>
-      </c>
       <c r="C125" s="28" t="s">
-        <v>385</v>
+        <v>382</v>
       </c>
       <c r="D125" s="14">
         <v>3</v>
       </c>
     </row>
-    <row r="126" spans="1:4" outlineLevel="1">
+    <row r="126" spans="1:4" hidden="1" outlineLevel="1">
       <c r="A126" s="4" t="s">
+        <v>263</v>
+      </c>
+      <c r="B126" s="15" t="s">
         <v>264</v>
       </c>
-      <c r="B126" s="15" t="s">
-        <v>265</v>
-      </c>
       <c r="C126" s="28" t="s">
-        <v>385</v>
+        <v>382</v>
       </c>
       <c r="D126" s="14">
         <v>3</v>
       </c>
     </row>
-    <row r="127" spans="1:4" outlineLevel="1">
+    <row r="127" spans="1:4" hidden="1" outlineLevel="1">
       <c r="A127" s="4" t="s">
+        <v>261</v>
+      </c>
+      <c r="B127" s="15" t="s">
         <v>262</v>
       </c>
-      <c r="B127" s="15" t="s">
-        <v>263</v>
-      </c>
       <c r="C127" s="28" t="s">
-        <v>385</v>
+        <v>382</v>
       </c>
       <c r="D127" s="14">
         <v>3</v>
       </c>
     </row>
-    <row r="128" spans="1:4" outlineLevel="1">
+    <row r="128" spans="1:4" hidden="1" outlineLevel="1">
       <c r="A128" s="4" t="s">
+        <v>257</v>
+      </c>
+      <c r="B128" s="15" t="s">
         <v>258</v>
       </c>
-      <c r="B128" s="15" t="s">
+      <c r="C128" s="28" t="s">
+        <v>382</v>
+      </c>
+      <c r="D128" s="14">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="129" spans="1:4" hidden="1" outlineLevel="1">
+      <c r="A129" s="4" t="s">
         <v>259</v>
       </c>
-      <c r="C128" s="28" t="s">
-        <v>385</v>
-      </c>
-      <c r="D128" s="14">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="129" spans="1:4" outlineLevel="1">
-      <c r="A129" s="4" t="s">
+      <c r="B129" s="15" t="s">
         <v>260</v>
       </c>
-      <c r="B129" s="15" t="s">
-        <v>261</v>
-      </c>
       <c r="C129" s="28" t="s">
-        <v>385</v>
+        <v>382</v>
       </c>
       <c r="D129" s="14">
         <v>3</v>
       </c>
     </row>
-    <row r="130" spans="1:4" outlineLevel="1">
+    <row r="130" spans="1:4" hidden="1" outlineLevel="1">
       <c r="A130" s="4" t="s">
+        <v>253</v>
+      </c>
+      <c r="B130" s="15" t="s">
         <v>254</v>
       </c>
-      <c r="B130" s="15" t="s">
+      <c r="C130" s="28" t="s">
+        <v>382</v>
+      </c>
+      <c r="D130" s="14">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="131" spans="1:4" hidden="1" outlineLevel="1">
+      <c r="A131" s="4" t="s">
         <v>255</v>
       </c>
-      <c r="C130" s="28" t="s">
-        <v>385</v>
-      </c>
-      <c r="D130" s="14">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="131" spans="1:4" outlineLevel="1">
-      <c r="A131" s="4" t="s">
+      <c r="B131" s="15" t="s">
         <v>256</v>
       </c>
-      <c r="B131" s="15" t="s">
-        <v>257</v>
-      </c>
       <c r="C131" s="28" t="s">
-        <v>385</v>
+        <v>382</v>
       </c>
       <c r="D131" s="14">
         <v>3</v>
       </c>
     </row>
-    <row r="132" spans="1:4" outlineLevel="1">
+    <row r="132" spans="1:4" hidden="1" outlineLevel="1">
       <c r="A132" s="4" t="s">
+        <v>247</v>
+      </c>
+      <c r="B132" s="15" t="s">
         <v>248</v>
       </c>
-      <c r="B132" s="15" t="s">
+      <c r="C132" s="28" t="s">
+        <v>382</v>
+      </c>
+      <c r="D132" s="14">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="133" spans="1:4" hidden="1" outlineLevel="1">
+      <c r="A133" s="4" t="s">
         <v>249</v>
       </c>
-      <c r="C132" s="28" t="s">
-        <v>385</v>
-      </c>
-      <c r="D132" s="14">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="133" spans="1:4" outlineLevel="1">
-      <c r="A133" s="4" t="s">
+      <c r="B133" s="15" t="s">
+        <v>251</v>
+      </c>
+      <c r="C133" s="28" t="s">
+        <v>382</v>
+      </c>
+      <c r="D133" s="14">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="134" spans="1:4" hidden="1" outlineLevel="1">
+      <c r="A134" s="4" t="s">
         <v>250</v>
       </c>
-      <c r="B133" s="15" t="s">
+      <c r="B134" s="15" t="s">
         <v>252</v>
       </c>
-      <c r="C133" s="28" t="s">
-        <v>385</v>
-      </c>
-      <c r="D133" s="14">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="134" spans="1:4" outlineLevel="1">
-      <c r="A134" s="4" t="s">
-        <v>251</v>
-      </c>
-      <c r="B134" s="15" t="s">
-        <v>253</v>
-      </c>
       <c r="C134" s="28" t="s">
-        <v>385</v>
+        <v>382</v>
       </c>
       <c r="D134" s="14">
         <v>3</v>
       </c>
     </row>
-    <row r="135" spans="1:4" outlineLevel="1">
+    <row r="135" spans="1:4" hidden="1" outlineLevel="1">
       <c r="A135" s="4" t="s">
+        <v>245</v>
+      </c>
+      <c r="B135" s="15" t="s">
         <v>246</v>
       </c>
-      <c r="B135" s="15" t="s">
-        <v>247</v>
-      </c>
       <c r="C135" s="28" t="s">
-        <v>385</v>
+        <v>382</v>
       </c>
       <c r="D135" s="14">
         <v>3</v>
       </c>
     </row>
-    <row r="136" spans="1:4" outlineLevel="1">
+    <row r="136" spans="1:4" hidden="1" outlineLevel="1">
       <c r="A136" s="4" t="s">
+        <v>239</v>
+      </c>
+      <c r="B136" s="15" t="s">
         <v>240</v>
       </c>
-      <c r="B136" s="15" t="s">
+      <c r="C136" s="28" t="s">
+        <v>382</v>
+      </c>
+      <c r="D136" s="14">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="137" spans="1:4" hidden="1" outlineLevel="1">
+      <c r="A137" s="4" t="s">
         <v>241</v>
       </c>
-      <c r="C136" s="28" t="s">
-        <v>385</v>
-      </c>
-      <c r="D136" s="14">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="137" spans="1:4" outlineLevel="1">
-      <c r="A137" s="4" t="s">
+      <c r="B137" s="15" t="s">
+        <v>243</v>
+      </c>
+      <c r="C137" s="28" t="s">
+        <v>382</v>
+      </c>
+      <c r="D137" s="14">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="138" spans="1:4" hidden="1" outlineLevel="1">
+      <c r="A138" s="4" t="s">
         <v>242</v>
       </c>
-      <c r="B137" s="15" t="s">
+      <c r="B138" s="15" t="s">
         <v>244</v>
       </c>
-      <c r="C137" s="28" t="s">
-        <v>385</v>
-      </c>
-      <c r="D137" s="14">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="138" spans="1:4" outlineLevel="1">
-      <c r="A138" s="4" t="s">
-        <v>243</v>
-      </c>
-      <c r="B138" s="15" t="s">
-        <v>245</v>
-      </c>
       <c r="C138" s="28" t="s">
-        <v>385</v>
+        <v>382</v>
       </c>
       <c r="D138" s="14">
         <v>3</v>
       </c>
     </row>
-    <row r="139" spans="1:4" outlineLevel="1">
+    <row r="139" spans="1:4" hidden="1" outlineLevel="1">
       <c r="A139" s="4" t="s">
+        <v>235</v>
+      </c>
+      <c r="B139" s="15" t="s">
         <v>236</v>
       </c>
-      <c r="B139" s="15" t="s">
+      <c r="C139" s="28" t="s">
+        <v>382</v>
+      </c>
+      <c r="D139" s="14">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="140" spans="1:4" hidden="1" outlineLevel="1">
+      <c r="A140" s="4" t="s">
         <v>237</v>
       </c>
-      <c r="C139" s="28" t="s">
-        <v>385</v>
-      </c>
-      <c r="D139" s="14">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="140" spans="1:4" outlineLevel="1">
-      <c r="A140" s="4" t="s">
+      <c r="B140" s="15" t="s">
         <v>238</v>
       </c>
-      <c r="B140" s="15" t="s">
-        <v>239</v>
-      </c>
       <c r="C140" s="28" t="s">
-        <v>385</v>
+        <v>382</v>
       </c>
       <c r="D140" s="14">
         <v>3</v>
       </c>
     </row>
-    <row r="141" spans="1:4" outlineLevel="1">
+    <row r="141" spans="1:4" hidden="1" outlineLevel="1">
       <c r="A141" s="4" t="s">
+        <v>229</v>
+      </c>
+      <c r="B141" s="15" t="s">
         <v>230</v>
       </c>
-      <c r="B141" s="15" t="s">
+      <c r="C141" s="28" t="s">
+        <v>382</v>
+      </c>
+      <c r="D141" s="14">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="142" spans="1:4" hidden="1" outlineLevel="1">
+      <c r="A142" s="4" t="s">
+        <v>232</v>
+      </c>
+      <c r="B142" s="15" t="s">
         <v>231</v>
       </c>
-      <c r="C141" s="28" t="s">
-        <v>385</v>
-      </c>
-      <c r="D141" s="14">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="142" spans="1:4" outlineLevel="1">
-      <c r="A142" s="4" t="s">
+      <c r="C142" s="28" t="s">
+        <v>382</v>
+      </c>
+      <c r="D142" s="14">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="143" spans="1:4" hidden="1" outlineLevel="1">
+      <c r="A143" s="4" t="s">
         <v>233</v>
       </c>
-      <c r="B142" s="15" t="s">
-        <v>232</v>
-      </c>
-      <c r="C142" s="28" t="s">
-        <v>385</v>
-      </c>
-      <c r="D142" s="14">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="143" spans="1:4" outlineLevel="1">
-      <c r="A143" s="4" t="s">
+      <c r="B143" s="15" t="s">
         <v>234</v>
       </c>
-      <c r="B143" s="15" t="s">
-        <v>235</v>
-      </c>
       <c r="C143" s="28" t="s">
-        <v>385</v>
+        <v>382</v>
       </c>
       <c r="D143" s="14">
         <v>3</v>
       </c>
     </row>
-    <row r="144" spans="1:4" outlineLevel="1">
+    <row r="144" spans="1:4" hidden="1" outlineLevel="1">
       <c r="A144" s="4" t="s">
+        <v>225</v>
+      </c>
+      <c r="B144" s="15" t="s">
         <v>226</v>
       </c>
-      <c r="B144" s="15" t="s">
+      <c r="C144" s="28" t="s">
+        <v>382</v>
+      </c>
+      <c r="D144" s="14">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="145" spans="1:4" hidden="1" outlineLevel="1">
+      <c r="A145" s="4" t="s">
         <v>227</v>
       </c>
-      <c r="C144" s="28" t="s">
-        <v>385</v>
-      </c>
-      <c r="D144" s="14">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="145" spans="1:4" outlineLevel="1">
-      <c r="A145" s="4" t="s">
+      <c r="B145" s="15" t="s">
         <v>228</v>
       </c>
-      <c r="B145" s="15" t="s">
-        <v>229</v>
-      </c>
       <c r="C145" s="28" t="s">
-        <v>385</v>
+        <v>382</v>
       </c>
       <c r="D145" s="14">
         <v>3</v>
       </c>
     </row>
-    <row r="146" spans="1:4" outlineLevel="1">
+    <row r="146" spans="1:4" hidden="1" outlineLevel="1">
       <c r="A146" s="4" t="s">
+        <v>219</v>
+      </c>
+      <c r="B146" s="15" t="s">
         <v>220</v>
       </c>
-      <c r="B146" s="15" t="s">
+      <c r="C146" s="28" t="s">
+        <v>382</v>
+      </c>
+      <c r="D146" s="14">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="147" spans="1:4" hidden="1" outlineLevel="1">
+      <c r="A147" s="4" t="s">
         <v>221</v>
       </c>
-      <c r="C146" s="28" t="s">
-        <v>385</v>
-      </c>
-      <c r="D146" s="14">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="147" spans="1:4" outlineLevel="1">
-      <c r="A147" s="4" t="s">
+      <c r="B147" s="15" t="s">
         <v>222</v>
       </c>
-      <c r="B147" s="15" t="s">
+      <c r="C147" s="28" t="s">
+        <v>382</v>
+      </c>
+      <c r="D147" s="14">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="148" spans="1:4" hidden="1" outlineLevel="1">
+      <c r="A148" s="4" t="s">
         <v>223</v>
       </c>
-      <c r="C147" s="28" t="s">
-        <v>385</v>
-      </c>
-      <c r="D147" s="14">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="148" spans="1:4" outlineLevel="1">
-      <c r="A148" s="4" t="s">
+      <c r="B148" s="15" t="s">
         <v>224</v>
       </c>
-      <c r="B148" s="15" t="s">
-        <v>225</v>
-      </c>
       <c r="C148" s="28" t="s">
-        <v>385</v>
+        <v>382</v>
       </c>
       <c r="D148" s="14">
         <v>3</v>
       </c>
     </row>
-    <row r="149" spans="1:4" outlineLevel="1">
+    <row r="149" spans="1:4" hidden="1" outlineLevel="1">
       <c r="A149" s="4" t="s">
+        <v>217</v>
+      </c>
+      <c r="B149" s="15" t="s">
         <v>218</v>
       </c>
-      <c r="B149" s="15" t="s">
-        <v>219</v>
-      </c>
       <c r="C149" s="28" t="s">
-        <v>385</v>
+        <v>382</v>
       </c>
       <c r="D149" s="14">
         <v>3</v>
       </c>
     </row>
-    <row r="150" spans="1:4" outlineLevel="1">
+    <row r="150" spans="1:4" hidden="1" outlineLevel="1">
       <c r="A150" s="16" t="s">
+        <v>215</v>
+      </c>
+      <c r="B150" s="15" t="s">
         <v>216</v>
       </c>
-      <c r="B150" s="15" t="s">
-        <v>217</v>
-      </c>
       <c r="C150" s="28" t="s">
-        <v>385</v>
+        <v>382</v>
       </c>
       <c r="D150" s="14">
         <v>3</v>
       </c>
     </row>
-    <row r="151" spans="1:4" outlineLevel="1">
+    <row r="151" spans="1:4" hidden="1" outlineLevel="1">
       <c r="A151" s="4" t="s">
+        <v>213</v>
+      </c>
+      <c r="B151" s="15" t="s">
         <v>214</v>
       </c>
-      <c r="B151" s="15" t="s">
-        <v>215</v>
-      </c>
       <c r="C151" s="28" t="s">
-        <v>385</v>
+        <v>382</v>
       </c>
       <c r="D151" s="14">
         <v>3</v>
       </c>
     </row>
-    <row r="152" spans="1:4" outlineLevel="1">
+    <row r="152" spans="1:4" hidden="1" outlineLevel="1">
       <c r="A152" s="4" t="s">
+        <v>211</v>
+      </c>
+      <c r="B152" s="18" t="s">
         <v>212</v>
       </c>
-      <c r="B152" s="18" t="s">
-        <v>213</v>
-      </c>
       <c r="C152" s="28" t="s">
-        <v>385</v>
+        <v>382</v>
       </c>
       <c r="D152" s="14">
         <v>3</v>
       </c>
     </row>
-    <row r="153" spans="1:4" outlineLevel="1">
+    <row r="153" spans="1:4" hidden="1" outlineLevel="1">
       <c r="A153" s="4" t="s">
+        <v>209</v>
+      </c>
+      <c r="B153" s="18" t="s">
         <v>210</v>
       </c>
-      <c r="B153" s="18" t="s">
-        <v>211</v>
-      </c>
       <c r="C153" s="28" t="s">
-        <v>385</v>
+        <v>382</v>
       </c>
       <c r="D153" s="14">
         <v>3</v>
       </c>
     </row>
-    <row r="154" spans="1:4" outlineLevel="1">
+    <row r="154" spans="1:4" hidden="1" outlineLevel="1">
       <c r="A154" s="4" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="B154" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="C154" s="3" t="s">
         <v>3</v>
@@ -5774,21 +5762,21 @@
         <v>1</v>
       </c>
     </row>
-    <row r="155" spans="1:4" outlineLevel="1">
+    <row r="155" spans="1:4" hidden="1" outlineLevel="1">
       <c r="A155" s="4" t="s">
+        <v>207</v>
+      </c>
+      <c r="B155" t="s">
         <v>208</v>
       </c>
-      <c r="B155" t="s">
-        <v>209</v>
-      </c>
-      <c r="C155" s="29" t="s">
-        <v>205</v>
+      <c r="C155" s="3" t="s">
+        <v>3</v>
       </c>
       <c r="D155" s="14">
         <v>1</v>
       </c>
     </row>
-    <row r="156" spans="1:4">
+    <row r="156" spans="1:4" collapsed="1">
       <c r="A156" s="21" t="s">
         <v>113</v>
       </c>
@@ -5797,7 +5785,7 @@
       </c>
       <c r="C156" s="23"/>
       <c r="D156" s="24" t="s">
-        <v>379</v>
+        <v>376</v>
       </c>
     </row>
     <row r="157" spans="1:4" outlineLevel="1">
@@ -5808,7 +5796,7 @@
         <v>50</v>
       </c>
       <c r="C157" s="3" t="s">
-        <v>385</v>
+        <v>382</v>
       </c>
       <c r="D157" s="14">
         <v>4</v>
@@ -5822,7 +5810,7 @@
         <v>52</v>
       </c>
       <c r="C158" s="3" t="s">
-        <v>385</v>
+        <v>382</v>
       </c>
       <c r="D158" s="14">
         <v>3</v>
@@ -5836,7 +5824,7 @@
         <v>54</v>
       </c>
       <c r="C159" s="3" t="s">
-        <v>385</v>
+        <v>382</v>
       </c>
       <c r="D159" s="14">
         <v>3</v>
@@ -5905,7 +5893,7 @@
       <c r="B164" t="s">
         <v>64</v>
       </c>
-      <c r="C164" s="30" t="s">
+      <c r="C164" s="29" t="s">
         <v>3</v>
       </c>
       <c r="D164" s="14">
@@ -5919,7 +5907,7 @@
       <c r="B165" t="s">
         <v>66</v>
       </c>
-      <c r="C165" s="30" t="s">
+      <c r="C165" s="29" t="s">
         <v>3</v>
       </c>
       <c r="D165" s="14">
@@ -5933,7 +5921,7 @@
       <c r="B166" t="s">
         <v>68</v>
       </c>
-      <c r="C166" s="30" t="s">
+      <c r="C166" s="29" t="s">
         <v>3</v>
       </c>
       <c r="D166" s="14">
@@ -5945,7 +5933,7 @@
         <v>69</v>
       </c>
       <c r="C167" s="3" t="s">
-        <v>385</v>
+        <v>382</v>
       </c>
       <c r="D167" s="14">
         <v>4</v>
@@ -5960,34 +5948,34 @@
       </c>
       <c r="C168" s="23"/>
       <c r="D168" s="24" t="s">
-        <v>379</v>
-      </c>
-    </row>
-    <row r="169" spans="1:4" outlineLevel="1">
+        <v>376</v>
+      </c>
+    </row>
+    <row r="169" spans="1:4" hidden="1" outlineLevel="1">
       <c r="C169" s="28" t="s">
-        <v>385</v>
+        <v>382</v>
       </c>
       <c r="D169" s="15"/>
     </row>
-    <row r="170" spans="1:4">
+    <row r="170" spans="1:4" collapsed="1">
       <c r="A170" s="21" t="s">
         <v>70</v>
       </c>
       <c r="B170" s="22" t="s">
-        <v>342</v>
+        <v>341</v>
       </c>
       <c r="C170" s="23"/>
       <c r="D170" s="24" t="s">
-        <v>379</v>
-      </c>
-    </row>
-    <row r="171" spans="1:4" outlineLevel="1">
+        <v>376</v>
+      </c>
+    </row>
+    <row r="171" spans="1:4" hidden="1" outlineLevel="1">
       <c r="C171" s="28" t="s">
-        <v>385</v>
+        <v>382</v>
       </c>
       <c r="D171" s="14"/>
     </row>
-    <row r="172" spans="1:4">
+    <row r="172" spans="1:4" collapsed="1">
       <c r="A172" s="21" t="s">
         <v>99</v>
       </c>
@@ -5996,16 +5984,16 @@
       </c>
       <c r="C172" s="23"/>
       <c r="D172" s="24" t="s">
-        <v>379</v>
-      </c>
-    </row>
-    <row r="173" spans="1:4" outlineLevel="1">
+        <v>376</v>
+      </c>
+    </row>
+    <row r="173" spans="1:4" hidden="1" outlineLevel="1">
       <c r="C173" s="28" t="s">
-        <v>385</v>
+        <v>382</v>
       </c>
       <c r="D173" s="14"/>
     </row>
-    <row r="174" spans="1:4">
+    <row r="174" spans="1:4" collapsed="1">
       <c r="A174" s="21" t="s">
         <v>115</v>
       </c>
@@ -6014,18 +6002,18 @@
       </c>
       <c r="C174" s="23"/>
       <c r="D174" s="24" t="s">
-        <v>379</v>
-      </c>
-    </row>
-    <row r="175" spans="1:4" outlineLevel="1">
+        <v>376</v>
+      </c>
+    </row>
+    <row r="175" spans="1:4" hidden="1" outlineLevel="1">
       <c r="A175" s="9"/>
       <c r="B175" s="9"/>
       <c r="C175" s="28" t="s">
-        <v>385</v>
+        <v>382</v>
       </c>
       <c r="D175" s="17"/>
     </row>
-    <row r="176" spans="1:4">
+    <row r="176" spans="1:4" collapsed="1">
       <c r="A176" s="21" t="s">
         <v>117</v>
       </c>
@@ -6034,18 +6022,18 @@
       </c>
       <c r="C176" s="23"/>
       <c r="D176" s="24" t="s">
-        <v>379</v>
-      </c>
-    </row>
-    <row r="177" spans="1:4" outlineLevel="1">
+        <v>376</v>
+      </c>
+    </row>
+    <row r="177" spans="1:4" hidden="1" outlineLevel="1">
       <c r="A177" s="9"/>
       <c r="B177" s="9"/>
       <c r="C177" s="28" t="s">
-        <v>385</v>
+        <v>382</v>
       </c>
       <c r="D177" s="17"/>
     </row>
-    <row r="178" spans="1:4">
+    <row r="178" spans="1:4" collapsed="1">
       <c r="A178" s="21" t="s">
         <v>119</v>
       </c>
@@ -6053,18 +6041,18 @@
         <v>120</v>
       </c>
       <c r="C178" s="24" t="s">
-        <v>379</v>
+        <v>376</v>
       </c>
       <c r="D178" s="24" t="s">
-        <v>379</v>
-      </c>
-    </row>
-    <row r="179" spans="1:4" outlineLevel="1">
+        <v>376</v>
+      </c>
+    </row>
+    <row r="179" spans="1:4" hidden="1" outlineLevel="1">
       <c r="A179" s="13" t="s">
+        <v>344</v>
+      </c>
+      <c r="B179" s="9" t="s">
         <v>345</v>
-      </c>
-      <c r="B179" s="9" t="s">
-        <v>346</v>
       </c>
       <c r="C179" s="10" t="s">
         <v>3</v>
@@ -6073,12 +6061,12 @@
         <v>1</v>
       </c>
     </row>
-    <row r="180" spans="1:4" outlineLevel="1">
+    <row r="180" spans="1:4" hidden="1" outlineLevel="1">
       <c r="A180" s="13" t="s">
+        <v>346</v>
+      </c>
+      <c r="B180" s="9" t="s">
         <v>347</v>
-      </c>
-      <c r="B180" s="9" t="s">
-        <v>348</v>
       </c>
       <c r="C180" s="10" t="s">
         <v>3</v>
@@ -6087,12 +6075,12 @@
         <v>1</v>
       </c>
     </row>
-    <row r="181" spans="1:4" outlineLevel="1">
+    <row r="181" spans="1:4" hidden="1" outlineLevel="1">
       <c r="A181" s="13" t="s">
+        <v>348</v>
+      </c>
+      <c r="B181" s="9" t="s">
         <v>349</v>
-      </c>
-      <c r="B181" s="9" t="s">
-        <v>350</v>
       </c>
       <c r="C181" s="10" t="s">
         <v>3</v>
@@ -6101,12 +6089,12 @@
         <v>1</v>
       </c>
     </row>
-    <row r="182" spans="1:4" outlineLevel="1">
+    <row r="182" spans="1:4" hidden="1" outlineLevel="1">
       <c r="A182" s="13" t="s">
-        <v>377</v>
+        <v>374</v>
       </c>
       <c r="B182" s="9" t="s">
-        <v>378</v>
+        <v>375</v>
       </c>
       <c r="C182" s="10" t="s">
         <v>3</v>
@@ -6115,26 +6103,26 @@
         <v>1</v>
       </c>
     </row>
-    <row r="183" spans="1:4" outlineLevel="1">
+    <row r="183" spans="1:4" hidden="1" outlineLevel="1">
       <c r="A183" s="13" t="s">
+        <v>350</v>
+      </c>
+      <c r="B183" s="9" t="s">
         <v>351</v>
       </c>
-      <c r="B183" s="9" t="s">
-        <v>352</v>
-      </c>
       <c r="C183" s="10" t="s">
-        <v>385</v>
+        <v>382</v>
       </c>
       <c r="D183" s="17">
         <v>2</v>
       </c>
     </row>
-    <row r="184" spans="1:4" outlineLevel="1">
+    <row r="184" spans="1:4" hidden="1" outlineLevel="1">
       <c r="A184" s="13" t="s">
+        <v>352</v>
+      </c>
+      <c r="B184" s="9" t="s">
         <v>353</v>
-      </c>
-      <c r="B184" s="9" t="s">
-        <v>354</v>
       </c>
       <c r="C184" s="10" t="s">
         <v>3</v>
@@ -6143,12 +6131,12 @@
         <v>1</v>
       </c>
     </row>
-    <row r="185" spans="1:4" outlineLevel="1">
+    <row r="185" spans="1:4" hidden="1" outlineLevel="1">
       <c r="A185" s="13" t="s">
+        <v>354</v>
+      </c>
+      <c r="B185" s="9" t="s">
         <v>355</v>
-      </c>
-      <c r="B185" s="9" t="s">
-        <v>356</v>
       </c>
       <c r="C185" s="10" t="s">
         <v>3</v>
@@ -6157,82 +6145,82 @@
         <v>1</v>
       </c>
     </row>
-    <row r="186" spans="1:4" outlineLevel="1">
+    <row r="186" spans="1:4" hidden="1" outlineLevel="1">
       <c r="A186" s="13" t="s">
+        <v>356</v>
+      </c>
+      <c r="B186" s="9" t="s">
         <v>357</v>
       </c>
-      <c r="B186" s="9" t="s">
-        <v>358</v>
-      </c>
       <c r="C186" s="10" t="s">
-        <v>385</v>
+        <v>382</v>
       </c>
       <c r="D186" s="17">
         <v>4</v>
       </c>
     </row>
-    <row r="187" spans="1:4" outlineLevel="1">
+    <row r="187" spans="1:4" hidden="1" outlineLevel="1">
       <c r="A187" s="13" t="s">
+        <v>358</v>
+      </c>
+      <c r="B187" s="9" t="s">
         <v>359</v>
       </c>
-      <c r="B187" s="9" t="s">
-        <v>360</v>
-      </c>
       <c r="C187" s="10" t="s">
-        <v>385</v>
+        <v>382</v>
       </c>
       <c r="D187" s="17">
         <v>2</v>
       </c>
     </row>
-    <row r="188" spans="1:4" outlineLevel="1">
+    <row r="188" spans="1:4" hidden="1" outlineLevel="1">
       <c r="A188" s="13" t="s">
+        <v>360</v>
+      </c>
+      <c r="B188" s="9" t="s">
         <v>361</v>
       </c>
-      <c r="B188" s="9" t="s">
-        <v>362</v>
-      </c>
       <c r="C188" s="10" t="s">
-        <v>385</v>
+        <v>382</v>
       </c>
       <c r="D188" s="17">
         <v>2</v>
       </c>
     </row>
-    <row r="189" spans="1:4" outlineLevel="1">
+    <row r="189" spans="1:4" hidden="1" outlineLevel="1">
       <c r="A189" s="13" t="s">
-        <v>364</v>
+        <v>363</v>
       </c>
       <c r="B189" s="9" t="s">
-        <v>363</v>
+        <v>362</v>
       </c>
       <c r="C189" s="10" t="s">
-        <v>385</v>
+        <v>382</v>
       </c>
       <c r="D189" s="17">
         <v>3</v>
       </c>
     </row>
-    <row r="190" spans="1:4" outlineLevel="1">
+    <row r="190" spans="1:4" hidden="1" outlineLevel="1">
       <c r="A190" s="13" t="s">
-        <v>386</v>
+        <v>383</v>
       </c>
       <c r="B190" s="9" t="s">
-        <v>387</v>
+        <v>384</v>
       </c>
       <c r="C190" s="10" t="s">
-        <v>385</v>
+        <v>382</v>
       </c>
       <c r="D190" s="17">
         <v>4</v>
       </c>
     </row>
-    <row r="191" spans="1:4" outlineLevel="1">
+    <row r="191" spans="1:4" hidden="1" outlineLevel="1">
       <c r="A191" s="13" t="s">
-        <v>388</v>
+        <v>385</v>
       </c>
       <c r="B191" s="9" t="s">
-        <v>392</v>
+        <v>389</v>
       </c>
       <c r="C191" s="10" t="s">
         <v>3</v>
@@ -6241,12 +6229,12 @@
         <v>2</v>
       </c>
     </row>
-    <row r="192" spans="1:4">
+    <row r="192" spans="1:4" hidden="1" outlineLevel="1">
       <c r="A192" s="4" t="s">
-        <v>389</v>
+        <v>386</v>
       </c>
       <c r="B192" t="s">
-        <v>390</v>
+        <v>387</v>
       </c>
       <c r="C192" s="3" t="s">
         <v>3</v>
@@ -6255,7 +6243,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="193" spans="1:4">
+    <row r="193" spans="1:4" collapsed="1">
       <c r="A193" s="21" t="s">
         <v>201</v>
       </c>
@@ -6264,7 +6252,7 @@
       </c>
       <c r="C193" s="23"/>
       <c r="D193" s="24" t="s">
-        <v>379</v>
+        <v>376</v>
       </c>
     </row>
     <row r="194" spans="1:4">
@@ -6279,22 +6267,22 @@
     </row>
     <row r="196" spans="1:4">
       <c r="A196" s="1" t="s">
-        <v>365</v>
+        <v>392</v>
       </c>
     </row>
     <row r="197" spans="1:4">
       <c r="A197" s="1" t="s">
-        <v>366</v>
+        <v>393</v>
       </c>
     </row>
     <row r="198" spans="1:4">
       <c r="A198" s="1" t="s">
-        <v>380</v>
+        <v>377</v>
       </c>
     </row>
     <row r="199" spans="1:4">
       <c r="A199" s="1" t="s">
-        <v>381</v>
+        <v>378</v>
       </c>
     </row>
     <row r="200" spans="1:4">
@@ -6304,22 +6292,22 @@
     </row>
     <row r="201" spans="1:4">
       <c r="A201" s="25" t="s">
-        <v>391</v>
+        <v>388</v>
       </c>
     </row>
     <row r="202" spans="1:4">
       <c r="A202" s="1" t="s">
-        <v>382</v>
+        <v>379</v>
       </c>
     </row>
     <row r="203" spans="1:4">
       <c r="A203" s="1" t="s">
-        <v>383</v>
+        <v>380</v>
       </c>
     </row>
     <row r="204" spans="1:4">
       <c r="A204" s="1" t="s">
-        <v>384</v>
+        <v>381</v>
       </c>
     </row>
     <row r="205" spans="1:4">

</xml_diff>